<commit_message>
fix : Crawler double issue
</commit_message>
<xml_diff>
--- a/naver_news_article_2022/미세먼지/20221113_미세먼지_.xlsx
+++ b/naver_news_article_2022/미세먼지/20221113_미세먼지_.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -639,17 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>연합뉴스</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[오늘날씨] 전국 돌풍·천둥 동반한 비…오후부터 기온 '뚝'</t>
+          <t>아침에 대부분 비 그쳐…강한 바람으로 체감온도↓</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862605</t>
+          <t>https://www.yna.co.kr/view/AKR20221113001900034?input=1195m</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>연합뉴스</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>아침에 대부분 비 그쳐…강한 바람으로 체감온도↓</t>
+          <t>서울시 '겨울철 종합대책' 가동…한파 관리도 "약자와의 동행"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.yna.co.kr/view/AKR20221113001900034?input=1195m</t>
+          <t>https://www.news1.kr/articles/4862209</t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>서울신문</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>서울시 '겨울철 종합대책' 가동…한파 관리도 "약자와의 동행"</t>
+          <t>가을비 이후 기온 뚝…‘수능 한파’는 없을 듯</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862209</t>
+          <t>https://www.seoul.co.kr/news/newsView.php?id=20221113500100&amp;wlog_tag3=naver</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>서울신문</t>
+          <t>아시아경제</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>가을비 이후 기온 뚝…‘수능 한파’는 없을 듯</t>
+          <t>[날씨]바람불어 체감온도 낮은 아침…경기·강원 1㎜ 비소식</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.seoul.co.kr/news/newsView.php?id=20221113500100&amp;wlog_tag3=naver</t>
+          <t>https://view.asiae.co.kr/article/2022111320071170342</t>
         </is>
       </c>
     </row>
@@ -727,17 +727,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>아시아경제</t>
+          <t>파이낸셜뉴스</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[날씨]바람불어 체감온도 낮은 아침…경기·강원 1㎜ 비소식</t>
+          <t>겨울 추위 본격 시작..북쪽 찬 공기 남하에 오후부터 기온 뚝</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://view.asiae.co.kr/article/2022111320071170342</t>
+          <t>http://www.fnnews.com/news/202211131050211030</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>파이낸셜뉴스</t>
+          <t>뉴시스</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>겨울 추위 본격 시작..북쪽 찬 공기 남하에 오후부터 기온 뚝</t>
+          <t>경기남부 비 그친 뒤 기온 '뚝'…낮 최고 12~14도</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>http://www.fnnews.com/news/202211131050211030</t>
+          <t>http://www.newsis.com/view/?id=NISX20221112_0002083796&amp;cID=10803&amp;pID=14000</t>
         </is>
       </c>
     </row>
@@ -771,17 +771,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>연합뉴스</t>
+          <t>JTBC</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[날씨] 바람 불고 추운 아침…중부지방 부슬비</t>
+          <t>비 그친 뒤 기온 '뚝'…서울 한낮 12도, 어제보다 10도↓</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.yna.co.kr/view/AKR20221113043300004?input=1195m</t>
+          <t>https://news.jtbc.co.kr/article/article.aspx?news_id=NB12091744</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>경기남부 비 그친 뒤 기온 '뚝'…낮 최고 12~14도</t>
+          <t>추수 끝나면 버려지는 농촌 폐비닐…"한달간 집중수거"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20221112_0002083796&amp;cID=10803&amp;pID=14000</t>
+          <t>http://www.newsis.com/view/?id=NISX20221112_0002083603&amp;cID=10201&amp;pID=10200</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>JTBC</t>
+          <t>연합뉴스</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>비 그친 뒤 기온 '뚝'…서울 한낮 12도, 어제보다 10도↓</t>
+          <t>[날씨] 바람 불고 추운 아침…중부지방 부슬비</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://news.jtbc.co.kr/article/article.aspx?news_id=NB12091744</t>
+          <t>https://www.yna.co.kr/view/AKR20221113043300004?input=1195m</t>
         </is>
       </c>
     </row>
@@ -837,17 +837,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>뉴시스</t>
+          <t>노컷뉴스</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>추수 끝나면 버려지는 농촌 폐비닐…"한달간 집중수거"</t>
+          <t>다중인파 장소 600여곳 특별점검…서울시, 겨울철 안전대책 강화</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20221112_0002083603&amp;cID=10201&amp;pID=10200</t>
+          <t>https://www.nocutnews.co.kr/news/5848281</t>
         </is>
       </c>
     </row>
@@ -859,17 +859,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>노컷뉴스</t>
+          <t>뉴시스</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>다중인파 장소 600여곳 특별점검…서울시, 겨울철 안전대책 강화</t>
+          <t>인천, 새벽까지 돌풍 동반 비…오후 찬 공기 남하해 '쌀쌀'</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.nocutnews.co.kr/news/5848281</t>
+          <t>http://www.newsis.com/view/?id=NISX20221112_0002083754&amp;cID=10802&amp;pID=14000</t>
         </is>
       </c>
     </row>
@@ -881,17 +881,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>뉴시스</t>
+          <t>코메디닷컴</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>인천, 새벽까지 돌풍 동반 비…오후 찬 공기 남하해 '쌀쌀'</t>
+          <t>갱년기 여성 '혈관 청소’, 염증 줄이는 음식은?</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20221112_0002083754&amp;cID=10802&amp;pID=14000</t>
+          <t>https://kormedi.com/?p=1542122</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>코메디닷컴</t>
+          <t>부산일보</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>갱년기 여성 '혈관 청소’, 염증 줄이는 음식은?</t>
+          <t>“아름다운 항구 도시 이름난 부산, 엑스포 유치에 유리… 행운 빈다”</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://kormedi.com/?p=1542122</t>
+          <t>https://www.busan.com/view/busan/view.php?code=2022111318453387516</t>
         </is>
       </c>
     </row>
@@ -925,17 +925,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>부산일보</t>
+          <t>프레시안</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>“아름다운 항구 도시 이름난 부산, 엑스포 유치에 유리… 행운 빈다”</t>
+          <t>국가 사라진 '10·29 참사'… 책임 부재 속 '선제적·실제적 조치' 눈길 끈 경기도</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.busan.com/view/busan/view.php?code=2022111318453387516</t>
+          <t>https://www.pressian.com/pages/articles/2022111317073822483?utm_source=naver&amp;utm_medium=search</t>
         </is>
       </c>
     </row>
@@ -947,17 +947,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>프레시안</t>
+          <t>뉴시스</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>국가 사라진 '10·29 참사'… 책임 부재 속 '선제적·실제적 조치' 눈길 끈 경기도</t>
+          <t>휴일 전북 낮 11~13도 어제보다 10도↓…찬바람까지</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.pressian.com/pages/articles/2022111317073822483?utm_source=naver&amp;utm_medium=search</t>
+          <t>http://www.newsis.com/view/?id=NISX20221113_0002083838&amp;cID=10808&amp;pID=10800</t>
         </is>
       </c>
     </row>
@@ -969,17 +969,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>뉴시스</t>
+          <t>디지털타임스</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>휴일 전북 낮 11~13도 어제보다 10도↓…찬바람까지</t>
+          <t>아태협 회장 구속에 정진석 "이재명 경기도-쌍방울과 대북송금·코인 3각 커넥션 밝혀야"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20221113_0002083838&amp;cID=10808&amp;pID=10800</t>
+          <t>http://www.dt.co.kr/contents.html?article_no=2022111302109958051001&amp;ref=naver</t>
         </is>
       </c>
     </row>
@@ -1123,17 +1123,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>bnt뉴스</t>
+          <t>보안뉴스</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>대형마트 휴무일,이마트·롯데마트·홈플러스·코스트코 ‘오늘 문여는 곳?’</t>
+          <t>구로구, ‘다기능 스마트폴’ 8곳에 추가 설치</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.bntnews.co.kr/article/view/bnt202211120041</t>
+          <t>http://www.boannews.com/media/view.asp?idx=111547&amp;kind=</t>
         </is>
       </c>
     </row>
@@ -1145,17 +1145,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>보안뉴스</t>
+          <t>bnt뉴스</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>구로구, ‘다기능 스마트폴’ 8곳에 추가 설치</t>
+          <t>대형마트 휴무일,이마트·롯데마트·홈플러스·코스트코 ‘오늘 문여는 곳?’</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>http://www.boannews.com/media/view.asp?idx=111547&amp;kind=</t>
+          <t>https://www.bntnews.co.kr/article/view/bnt202211120041</t>
         </is>
       </c>
     </row>
@@ -1211,17 +1211,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>디지털타임스</t>
+          <t>오마이뉴스</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>아태협 회장 구속에 정진석 "이재명 경기도-쌍방울과 대북송금·코인 3각 커넥션 밝혀야"</t>
+          <t>[홍성] 쌀쌀한 주말... "비 그치면 추워져"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>http://www.dt.co.kr/contents.html?article_no=2022111302109958051001&amp;ref=naver</t>
+          <t>http://www.ohmynews.com/NWS_Web/View/at_pg.aspx?CNTN_CD=A0002880174&amp;CMPT_CD=P0010&amp;utm_source=naver&amp;utm_medium=newsearch&amp;utm_campaign=naver_news</t>
         </is>
       </c>
     </row>
@@ -1233,17 +1233,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>오마이뉴스</t>
+          <t>조세일보</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[홍성] 쌀쌀한 주말... "비 그치면 추워져"</t>
+          <t>[날씨] 전국 흐리고 오전까지 비…그친 뒤 기온 뚝</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>http://www.ohmynews.com/NWS_Web/View/at_pg.aspx?CNTN_CD=A0002880174&amp;CMPT_CD=P0010&amp;utm_source=naver&amp;utm_medium=newsearch&amp;utm_campaign=naver_news</t>
+          <t>http://www.joseilbo.com/news/news_read.php?uid=470933&amp;class=33&amp;grp=</t>
         </is>
       </c>
     </row>
@@ -1255,17 +1255,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>조세일보</t>
+          <t>JTBC</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[날씨] 전국 흐리고 오전까지 비…그친 뒤 기온 뚝</t>
+          <t>[날씨] 오후부터 기온 '뚝'…낮 최고 서울·광주 13도</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>http://www.joseilbo.com/news/news_read.php?uid=470933&amp;class=33&amp;grp=</t>
+          <t>https://news.jtbc.co.kr/article/article.aspx?news_id=NB12091756</t>
         </is>
       </c>
     </row>
@@ -1277,17 +1277,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>JTBC</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[날씨] 오후부터 기온 '뚝'…낮 최고 서울·광주 13도</t>
+          <t>[오늘의 날씨]전북(13일, 일)…비 그친 후 기온 떨어져</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://news.jtbc.co.kr/article/article.aspx?news_id=NB12091756</t>
+          <t>https://www.news1.kr/articles/4862503</t>
         </is>
       </c>
     </row>
@@ -1299,17 +1299,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>일요신문</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[오늘의 날씨]전북(13일, 일)…비 그친 후 기온 떨어져</t>
+          <t>[김해시] 대한민국 지방자치경영대전 사상 최초 수상 外</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862503</t>
+          <t>https://ilyo.co.kr/?ac=article_view&amp;entry_id=440522</t>
         </is>
       </c>
     </row>
@@ -1321,17 +1321,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>남도일보</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>날씨 예보, 내일 날씨 전국 쌀쌀...서울 낮 최고 14도</t>
+          <t>[오늘의 날씨] 울산(13일, 일)…흐리고 오후 한때 비</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>http://www.namdonews.com/news/articleView.html?idxno=702899</t>
+          <t>https://www.news1.kr/articles/4862523</t>
         </is>
       </c>
     </row>
@@ -1343,17 +1343,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>일요신문</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[김해시] 대한민국 지방자치경영대전 사상 최초 수상 外</t>
+          <t>[오늘의 날씨]대구·경북(13일, 일)…낮 17도 안팎, 비 온 뒤 기온 '뚝'</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://ilyo.co.kr/?ac=article_view&amp;entry_id=440522</t>
+          <t>https://www.news1.kr/articles/4862535</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>서울경제</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[오늘의 날씨] 울산(13일, 일)…흐리고 오후 한때 비</t>
+          <t>“함께 웃으면서 걸으니 저절로 힐링되네요”</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862523</t>
+          <t>https://www.sedaily.com/NewsView/26DLZ3TAG4</t>
         </is>
       </c>
     </row>
@@ -1409,17 +1409,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>서울경제</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>“함께 웃으면서 걸으니 저절로 힐링되네요”</t>
+          <t>[오늘의 날씨]부산·경남(13일, 일)…해안가 너울 '주의'</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.sedaily.com/NewsView/26DLZ3TAG4</t>
+          <t>https://www.news1.kr/articles/4862525</t>
         </is>
       </c>
     </row>
@@ -1431,17 +1431,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>남도일보</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[오늘의 날씨]부산·경남(13일, 일)…해안가 너울 '주의'</t>
+          <t>날씨 예보, 내일 날씨 전국 쌀쌀...서울 낮 최고 14도</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862525</t>
+          <t>http://www.namdonews.com/news/articleView.html?idxno=702899</t>
         </is>
       </c>
     </row>
@@ -1453,17 +1453,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>경남매일신문</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>김해시， 지방자치경영대전 최우수 수상</t>
+          <t>[오늘의 날씨] 대전·충남(13일, 일)…대체로 흐림, 새벽 우박·비</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>http://www.gnmaeil.com/news/articleView.html?idxno=507467</t>
+          <t>https://www.news1.kr/articles/4862592</t>
         </is>
       </c>
     </row>
@@ -1475,17 +1475,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>UPI뉴스</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[오늘의 날씨] 대전·충남(13일, 일)…대체로 흐림, 새벽 우박·비</t>
+          <t>비 온 뒤 기온 '뚝'… 15일 아침 영하권</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862592</t>
+          <t>http://www.upinews.kr/newsView/upi202211130020</t>
         </is>
       </c>
     </row>
@@ -1497,17 +1497,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>UPI뉴스</t>
+          <t>아시아경제</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>비 온 뒤 기온 '뚝'… 15일 아침 영하권</t>
+          <t>[내일날씨]전국에 구름 많고 쌀쌀…아침 최저기온 3~11도</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>http://www.upinews.kr/newsView/upi202211130020</t>
+          <t>https://view.asiae.co.kr/article/2022111309100265500</t>
         </is>
       </c>
     </row>
@@ -1519,17 +1519,17 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>아시아경제</t>
+          <t>경인일보</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[내일날씨]전국에 구름 많고 쌀쌀…아침 최저기온 3~11도</t>
+          <t>[나의 의정일지] 국중범 경기도의회 운영위·여성가족위원</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://view.asiae.co.kr/article/2022111309100265500</t>
+          <t>http://www.kyeongin.com/main/view.php?key=20221109010001691</t>
         </is>
       </c>
     </row>
@@ -1541,17 +1541,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>경인일보</t>
+          <t>중부일보</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>[나의 의정일지] 국중범 경기도의회 운영위·여성가족위원</t>
+          <t>무관심에 막힌 보행로…이동약자들 큰 불편</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>http://www.kyeongin.com/main/view.php?key=20221109010001691</t>
+          <t>http://www.joongboo.com/news/articleView.html?idxno=363565992</t>
         </is>
       </c>
     </row>
@@ -1568,12 +1568,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>[오늘의 날씨]대구·경북(13일, 일)…낮 17도 안팎, 비 온 뒤 기온 '뚝'</t>
+          <t>[오늘의 날씨] 강원(13일, 일)…비 그치면 기온 뚝· 산간 고지대 최대 5㎝ 눈</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862535</t>
+          <t>https://www.news1.kr/articles/4862518</t>
         </is>
       </c>
     </row>
@@ -1585,17 +1585,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>매일일보</t>
+          <t>에너지경제</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>강원도, 횡성형 일자리 성과물 '포트로' 100% 납품</t>
+          <t>우편배달용 초소형 전기 화물차, 포트로 100% 납품</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>http://www.m-i.kr/news/articleView.html?idxno=963826</t>
+          <t>https://www.ekn.kr/web/view.php?key=20221113010002249</t>
         </is>
       </c>
     </row>
@@ -1607,17 +1607,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>중부일보</t>
+          <t>매일일보</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>무관심에 막힌 보행로…이동약자들 큰 불편</t>
+          <t>시멘트 시설 '형평성' 논란 커진다</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>http://www.joongboo.com/news/articleView.html?idxno=363565992</t>
+          <t>http://www.m-i.kr/news/articleView.html?idxno=963779</t>
         </is>
       </c>
     </row>
@@ -1629,17 +1629,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>신아일보</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>[오늘의 날씨] 강원(13일, 일)…비 그치면 기온 뚝· 산간 고지대 최대 5㎝ 눈</t>
+          <t>[오늘날씨] 전국 흐리고 비… 낮최고 22도</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862518</t>
+          <t>http://www.shinailbo.co.kr/news/articleView.html?idxno=1622309</t>
         </is>
       </c>
     </row>
@@ -1651,17 +1651,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>매일일보</t>
+          <t>MTN</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>시멘트 시설 '형평성' 논란 커진다</t>
+          <t>한물 갔다더니 인테리어 필수템됐네?…'중문'의 재발견, 왜</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>http://www.m-i.kr/news/articleView.html?idxno=963779</t>
+          <t>https://news.mtn.co.kr/news-detail/2022111309161947380</t>
         </is>
       </c>
     </row>
@@ -1673,17 +1673,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>MTN</t>
+          <t>컨슈머타임스</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>한물 갔다더니 인테리어 필수템됐네?…'중문'의 재발견, 왜</t>
+          <t>인천시, 도시숲 더욱 푸르러 지도록 '숲가꾸기' 나서</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://news.mtn.co.kr/news-detail/2022111309161947380</t>
+          <t>https://www.cstimes.com/news/articleView.html?idxno=519173</t>
         </is>
       </c>
     </row>
@@ -1695,17 +1695,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>컨슈머타임스</t>
+          <t>경북일보</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>인천시, 도시숲 더욱 푸르러 지도록 '숲가꾸기' 나서</t>
+          <t>경산시자원봉사센터, 보행자의 날 게릴라 캠페인 진행</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://www.cstimes.com/news/articleView.html?idxno=519173</t>
+          <t>http://www.kyongbuk.co.kr/news/articleView.html?idxno=2116794</t>
         </is>
       </c>
     </row>
@@ -1717,17 +1717,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>경북일보</t>
+          <t>뉴스프리존</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>경산시자원봉사센터, 보행자의 날 게릴라 캠페인 진행</t>
+          <t>창원시, 동절기 종합대책 추진…안전하고 따뜻한 겨울나기 돌입</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>http://www.kyongbuk.co.kr/news/articleView.html?idxno=2116794</t>
+          <t>http://www.newsfreezone.co.kr/news/articleView.html?idxno=423787</t>
         </is>
       </c>
     </row>
@@ -1739,17 +1739,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>뉴스프리존</t>
+          <t>동양일보</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>창원시, 동절기 종합대책 추진…안전하고 따뜻한 겨울나기 돌입</t>
+          <t>기자수첩/ 국내 1호 음성LNG발전소, 환경이 우선이다</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>http://www.newsfreezone.co.kr/news/articleView.html?idxno=423787</t>
+          <t>http://www.dynews.co.kr/news/articleView.html?idxno=680334</t>
         </is>
       </c>
     </row>
@@ -1761,17 +1761,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>동양일보</t>
+          <t>데일리한국</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>기자수첩/ 국내 1호 음성LNG발전소, 환경이 우선이다</t>
+          <t>[오늘(13일)의 날씨] 전국 흐리고 비...수도권 최대 60mm</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>http://www.dynews.co.kr/news/articleView.html?idxno=680334</t>
+          <t>https://daily.hankooki.com/news/articleView.html?idxno=892659</t>
         </is>
       </c>
     </row>
@@ -1783,17 +1783,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>데일리한국</t>
+          <t>뉴데일리</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[오늘(13일)의 날씨] 전국 흐리고 비...수도권 최대 60mm</t>
+          <t>[진경수의 산이야기] 제비봉 절경, 사람 손길 만큼 몸살 앓아…안타까움 ‘가득’</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>https://daily.hankooki.com/news/articleView.html?idxno=892659</t>
+          <t>https://cc.newdaily.co.kr/site/data/html/2022/11/13/2022111300039.html</t>
         </is>
       </c>
     </row>
@@ -1805,17 +1805,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>뉴데일리</t>
+          <t>시민일보</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[진경수의 산이야기] 제비봉 절경, 사람 손길 만큼 몸살 앓아…안타까움 ‘가득’</t>
+          <t>인천시 계양구, 산불조심기간 산불예방 총력 대응</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>https://cc.newdaily.co.kr/site/data/html/2022/11/13/2022111300039.html</t>
+          <t>https://www.siminilbo.co.kr/news/newsview.php?ncode=1160278866116654</t>
         </is>
       </c>
     </row>
@@ -1827,17 +1827,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>시민일보</t>
+          <t>EBN</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>인천시 계양구, 산불조심기간 산불예방 총력 대응</t>
+          <t>[내일(14일) 날씨] 아침 최저 3~11도…전국에 구름 많아</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>https://www.siminilbo.co.kr/news/newsview.php?ncode=1160278866116654</t>
+          <t>https://www.ebn.co.kr/news/view/1554627/?sc=Naver</t>
         </is>
       </c>
     </row>
@@ -1849,17 +1849,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>EBN</t>
+          <t>에너지경제</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>[내일(14일) 날씨] 아침 최저 3~11도…전국에 구름 많아</t>
+          <t>[중후장대, 넷제로에 도전] 장태선 화학연 단장 "국내 산업계, CCUS 기술 개발 드라이브 걸어야"</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>https://www.ebn.co.kr/news/view/1554627/?sc=Naver</t>
+          <t>https://www.ekn.kr/web/view.php?key=20221112010002201</t>
         </is>
       </c>
     </row>
@@ -1871,17 +1871,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>신아일보</t>
+          <t>울산제일일보</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>[오늘날씨] 전국 흐리고 비… 낮최고 22도</t>
+          <t>"경윳값 너무 비싸" 디젤차 인기 '뚝'</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>http://www.shinailbo.co.kr/news/articleView.html?idxno=1622309</t>
+          <t>http://www.ujeil.com/news/articleView.html?idxno=316012</t>
         </is>
       </c>
     </row>
@@ -1893,17 +1893,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>에너지경제</t>
+          <t>충북일보</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[중후장대, 넷제로에 도전] 장태선 화학연 단장 "국내 산업계, CCUS 기술 개발 드라이브 걸어야"</t>
+          <t>&lt;날씨&gt;14일 충북 추운 날씨</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://www.ekn.kr/web/view.php?key=20221112010002201</t>
+          <t>https://www.inews365.com/news/article.html?no=739354</t>
         </is>
       </c>
     </row>
@@ -1915,17 +1915,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>울산제일일보</t>
+          <t>중도일보</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>"경윳값 너무 비싸" 디젤차 인기 '뚝'</t>
+          <t>[날씨] 낮 기온 '뚝' 전국이 쌀쌀… 대전 낮 최고 15도</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>http://www.ujeil.com/news/articleView.html?idxno=316012</t>
+          <t>http://www.joongdo.co.kr/web/view.php?key=20221113010003756</t>
         </is>
       </c>
     </row>
@@ -1937,17 +1937,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>충북일보</t>
+          <t>에너지경제</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>&lt;날씨&gt;14일 충북 추운 날씨</t>
+          <t>‘2022 기상기후산업박람회’ 성황…온라인 전시관 총 10만명 방문</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://www.inews365.com/news/article.html?no=739354</t>
+          <t>https://www.ekn.kr/web/view.php?key=20221112010002175</t>
         </is>
       </c>
     </row>
@@ -1959,17 +1959,17 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>중도일보</t>
+          <t>동양일보</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[날씨] 낮 기온 '뚝' 전국이 쌀쌀… 대전 낮 최고 15도</t>
+          <t>비 온 뒤 '쌀쌀'...충청권 낮 최고 15도</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>http://www.joongdo.co.kr/web/view.php?key=20221113010003756</t>
+          <t>http://www.dynews.co.kr/news/articleView.html?idxno=680405</t>
         </is>
       </c>
     </row>
@@ -1981,17 +1981,17 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>에너지경제</t>
+          <t>스카이데일리</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>‘2022 기상기후산업박람회’ 성황…온라인 전시관 총 10만명 방문</t>
+          <t>[날씨] 전국 대체로 흐리고 경기·전라 빗방울… 강원산지 바람</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://www.ekn.kr/web/view.php?key=20221112010002175</t>
+          <t>http://www.skyedaily.com/news/news_view.html?ID=173292</t>
         </is>
       </c>
     </row>
@@ -2003,17 +2003,17 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>동양일보</t>
+          <t>매일일보</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>비 온 뒤 '쌀쌀'...충청권 낮 최고 15도</t>
+          <t>대방 '충남내포신도시 디에트르' 1474가구 분양…'학세권' 강점</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>http://www.dynews.co.kr/news/articleView.html?idxno=680405</t>
+          <t>http://www.m-i.kr/news/articleView.html?idxno=963603</t>
         </is>
       </c>
     </row>
@@ -2025,17 +2025,17 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>스카이데일리</t>
+          <t>제주교통복지신문</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[날씨] 전국 대체로 흐리고 경기·전라 빗방울… 강원산지 바람</t>
+          <t>[TW포토] 제주시 신대로 녹색쌈지 도시숲 안내판</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>http://www.skyedaily.com/news/news_view.html?ID=173292</t>
+          <t>https://www.jejutwn.com/news/article.html?no=152366</t>
         </is>
       </c>
     </row>
@@ -2047,17 +2047,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>매일일보</t>
+          <t>오피니언뉴스</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>대방 '충남내포신도시 디에트르' 1474가구 분양…'학세권' 강점</t>
+          <t>[모빌리티 세상읽기] 전기차 전환에 브레이크 밟는 EU와 유로7, 왜?</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>http://www.m-i.kr/news/articleView.html?idxno=963603</t>
+          <t>http://www.opinionnews.co.kr/news/articleView.html?idxno=76287</t>
         </is>
       </c>
     </row>
@@ -2069,17 +2069,17 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>제주교통복지신문</t>
+          <t>건설타임즈</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>[TW포토] 제주시 신대로 녹색쌈지 도시숲 안내판</t>
+          <t>'e편한세상 탕정 퍼스트드림' 13일까지 예비당첨자 서류 접수</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://www.jejutwn.com/news/article.html?no=152366</t>
+          <t>http://www.constimes.co.kr/news/articleView.html?idxno=235541</t>
         </is>
       </c>
     </row>
@@ -2091,17 +2091,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>오피니언뉴스</t>
+          <t>핀포인트뉴스</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>[모빌리티 세상읽기] 전기차 전환에 브레이크 밟는 EU와 유로7, 왜?</t>
+          <t>비에이치아이, 주가 60% 이상 뛰어…무슨 이유 있나?</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>http://www.opinionnews.co.kr/news/articleView.html?idxno=76287</t>
+          <t>http://www.pinpointnews.co.kr/news/articleView.html?idxno=154720</t>
         </is>
       </c>
     </row>
@@ -2113,17 +2113,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>건설타임즈</t>
+          <t>남도일보</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>'e편한세상 탕정 퍼스트드림' 13일까지 예비당첨자 서류 접수</t>
+          <t>순천시, 어린이체육관 '주민 참여 디자인' 공모…논란 재점화 되나</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>http://www.constimes.co.kr/news/articleView.html?idxno=235541</t>
+          <t>http://www.namdonews.com/news/articleView.html?idxno=702808</t>
         </is>
       </c>
     </row>
@@ -2135,17 +2135,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>중부일보</t>
+          <t>전북의소리</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>[오늘날씨] 전국 흐리고 비… 수원 9∼14도·인천 7∼13도</t>
+          <t>[오늘의 전북 날씨] 오전까지 '빗방울'...한낮 기온 '뚝'</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>http://www.joongboo.com/news/articleView.html?idxno=363565917</t>
+          <t>http://www.jbsori.com/news/articleView.html?idxno=9974</t>
         </is>
       </c>
     </row>
@@ -2157,17 +2157,17 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>핀포인트뉴스</t>
+          <t>더퍼블릭</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>비에이치아이, 주가 60% 이상 뛰어…무슨 이유 있나?</t>
+          <t>'대북 송금 의혹' 아태협 안모 회장 구속…法 “혐의 소명·도주 우려”</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>http://www.pinpointnews.co.kr/news/articleView.html?idxno=154720</t>
+          <t>https://thepublic.kr/news/view/1065612316421926</t>
         </is>
       </c>
     </row>
@@ -2179,17 +2179,17 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>남도일보</t>
+          <t>신아일보</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>순천시, 어린이체육관 '주민 참여 디자인' 공모…논란 재점화 되나</t>
+          <t>동작구 실내놀이터 상도3동점 14일 개소…날씨 걱정없이 이용하세요</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>http://www.namdonews.com/news/articleView.html?idxno=702808</t>
+          <t>http://www.shinailbo.co.kr/news/articleView.html?idxno=1622402</t>
         </is>
       </c>
     </row>
@@ -2201,17 +2201,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>전북의소리</t>
+          <t>중앙신문</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>[오늘의 전북 날씨] 오전까지 '빗방울'...한낮 기온 '뚝'</t>
+          <t>[오늘의 날씨] 경기·인천(13일, 일)…기온 뚝 떨어져</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>http://www.jbsori.com/news/articleView.html?idxno=9974</t>
+          <t>http://www.joongang.tv/news/articleView.html?idxno=57975</t>
         </is>
       </c>
     </row>
@@ -2223,17 +2223,17 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>충청매일</t>
+          <t>전북의소리</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>순천향대, 연구역량·업적 빛났다</t>
+          <t>[오늘의 전북 날씨] 오전까지 '빗방울'...한낮 기온 '뚝'</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>http://www.ccdn.co.kr/news/articleView.html?idxno=789555</t>
+          <t>http://www.jbsori.com/news/articleView.html?idxno=9974</t>
         </is>
       </c>
     </row>
@@ -2333,17 +2333,17 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>SR타임스</t>
+          <t>충청매일</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>[오늘 날씨 및 내일 날씨] 가을비 그친 뒤 기온 뚝↓...서울 최저기온 9도...종일 찬바람</t>
+          <t>공주시 월송동, 가을철 산불조심 홍보 캠페인 실시</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>http://www.srtimes.kr/news/articleView.html?idxno=123576</t>
+          <t>http://www.ccdn.co.kr/news/articleView.html?idxno=789608</t>
         </is>
       </c>
     </row>
@@ -2421,17 +2421,17 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>충청매일</t>
+          <t>SR타임스</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>공주시 월송동, 가을철 산불조심 홍보 캠페인 실시</t>
+          <t>[오늘 날씨 및 내일 날씨] 가을비 그친 뒤 기온 뚝↓...서울 최저기온 9도...종일 찬바람</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>http://www.ccdn.co.kr/news/articleView.html?idxno=789608</t>
+          <t>http://www.srtimes.kr/news/articleView.html?idxno=123576</t>
         </is>
       </c>
     </row>
@@ -2443,17 +2443,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>아시아투데이</t>
+          <t>브릿지경제</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>순천향대 연구자 12명, 최상위 2% 세계 과학자 리스트에 선정</t>
+          <t>순천향대, 최상위 2% 세계 과학자 리스트 이름 올려</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>https://www.asiatoday.co.kr/view.php?key=20221113010006573</t>
+          <t>https://www.viva100.com/main/view.php?key=20221113010003503</t>
         </is>
       </c>
     </row>
@@ -2465,17 +2465,17 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>중부매일</t>
+          <t>아시아투데이</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>순천향대, 2021 논문 피인용 수 기준 글로벌 최상위 2%</t>
+          <t>순천향대 연구자 12명, 최상위 2% 세계 과학자 리스트에 선정</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>http://www.jbnews.com/news/articleView.html?idxno=1376141</t>
+          <t>https://www.asiatoday.co.kr/view.php?key=20221113010006573</t>
         </is>
       </c>
     </row>
@@ -2487,17 +2487,17 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>충청일보</t>
+          <t>중부매일</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>순천향대, 세계 과학자 리스트에 이름 올려</t>
+          <t>순천향대, 2021 논문 피인용 수 기준 글로벌 최상위 2%</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://www.ccdailynews.com/news/articleView.html?idxno=2166707</t>
+          <t>http://www.jbnews.com/news/articleView.html?idxno=1376141</t>
         </is>
       </c>
     </row>
@@ -2509,17 +2509,17 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>브릿지경제</t>
+          <t>충청일보</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>순천향대, 최상위 2% 세계 과학자 리스트 이름 올려</t>
+          <t>순천향대, 세계 과학자 리스트에 이름 올려</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://www.viva100.com/main/view.php?key=20221113010003503</t>
+          <t>https://www.ccdailynews.com/news/articleView.html?idxno=2166707</t>
         </is>
       </c>
     </row>
@@ -2575,17 +2575,17 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>뉴시스</t>
+          <t>국제뉴스</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>추수 끝나면 버려지는 농촌 폐비닐…"한달간 집중수거"</t>
+          <t>[오늘의 날씨] 전국 흐리고 곳곳 가을비 소식 '오후부터 기온 뚝' 최고 22도...미세먼지 좋음</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20221112_0002083603&amp;cID=10201&amp;pID=10200</t>
+          <t>https://www.gukjenews.com/news/articleView.html?idxno=2591183</t>
         </is>
       </c>
     </row>
@@ -2597,17 +2597,17 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>뉴스1</t>
+          <t>뉴시스</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>환경부, 내달 중순까지 폐비닐·폐농약용기 등 영농폐기물 집중 수거</t>
+          <t>전국 곳곳 오전까지 비 소식…오후부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://www.news1.kr/articles/4862310</t>
+          <t>http://www.newsis.com/view/?id=NISX20221112_0002083801&amp;cID=10201&amp;pID=10200</t>
         </is>
       </c>
     </row>
@@ -2619,17 +2619,17 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>헤럴드경제</t>
+          <t>뉴스1</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>민관 합동으로 영농폐기물 집중 수거한다</t>
+          <t>[오늘날씨] 전국 돌풍·천둥 동반한 비…오후부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>http://news.heraldcorp.com/view.php?ud=20221113000040</t>
+          <t>https://www.news1.kr/articles/4862605</t>
         </is>
       </c>
     </row>
@@ -2641,17 +2641,17 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>이데일리</t>
+          <t>채널A</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>영농폐기물 집중수거기간 한달간 운영…우수 지자체 포상</t>
+          <t>전국 흐리고 비…오후부터 기온 떨어져 '쌀쌀'</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>http://www.edaily.co.kr/news/newspath.asp?newsid=01436646632525392</t>
+          <t>http://www.ichannela.com/news/main/news_detailPage.do?publishId=000000322274</t>
         </is>
       </c>
     </row>
@@ -2663,17 +2663,17 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>이투데이</t>
+          <t>일요신문</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>영농 폐비닐 수거보상금 지원단가 kg당 10→20원으로 인상</t>
+          <t>[날씨] 오늘날씨, 일요일 전국 흐리고 '비'…많은 곳 '60㎜'</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>https://www.etoday.co.kr/news/view/2191814</t>
+          <t>http://ilyo.co.kr/?ac=article_view&amp;entry_id=440621</t>
         </is>
       </c>
     </row>
@@ -2685,17 +2685,17 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>전자신문</t>
+          <t>아시아투데이</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>민관, 영농폐기물 집중 수거…“보상금 확대, 재활용시설 확충”</t>
+          <t>[오늘 날씨] 전국 아침까지 비…낮부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>https://www.etnews.com/20221113000027</t>
+          <t>https://www.asiatoday.co.kr/view.php?key=20221113010006621</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>데일리안</t>
+          <t>비욘드포스트</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>환경부, 내달 16일까지 방치된 폐비닐·폐농약용기 집중 수거</t>
+          <t>[날씨] 일요일, 전국 오전까지 비…오후부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>https://www.dailian.co.kr/news/view/1172571/?sc=Naver</t>
+          <t>http://www.beyondpost.co.kr/view.php?ud=20221113083103436046a9e4dd7f_30</t>
         </is>
       </c>
     </row>
@@ -2729,17 +2729,17 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>뉴시스</t>
+          <t>딜라이트닷넷</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>찬공기 유입에 내일 아침 쌀쌀…구름 많고 안개</t>
+          <t>[오늘날씨] 아침에 대부분 비 그쳐...오후부터 기온 뚝 떨어져</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>http://www.newsis.com/view/?id=NISX20221113_0002084142&amp;cID=10201&amp;pID=10200</t>
+          <t>http://www.delighti.co.kr/news/articleView.html?idxno=41990</t>
         </is>
       </c>
     </row>
@@ -2751,17 +2751,17 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>세계일보</t>
+          <t>이코노뉴스</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>[내일날씨] 전국 구름 많은 가운데 13일보다 5∼10도 더 떨어져</t>
+          <t>[오늘 날씨] 전국 곳곳 오전까지 가을비…오후부터 기온 '뚝'-바람 불어 체감온도 더 낮아</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>http://www.segye.com/content/html/2022/11/13/20221113508264.html?OutUrl=naver</t>
+          <t>http://www.econonews.co.kr/news/articleView.html?idxno=266278</t>
         </is>
       </c>
     </row>
@@ -2773,17 +2773,17 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>머니S</t>
+          <t>이코노믹리뷰</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>[내일 날씨] 전국 구름 많고 기온 '뚝'… 서울 최고기온 14도</t>
+          <t>[오늘날씨] 전국 오전까지 비 소식...오후부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>http://moneys.mt.co.kr/news/mwView.php?no=2022111315372838730</t>
+          <t>https://www.econovill.com/news/articleView.html?idxno=595144</t>
         </is>
       </c>
     </row>
@@ -2795,17 +2795,17 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>bnt뉴스</t>
+          <t>핀포인트뉴스</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>내일날씨, 찬 바람 기온 ‘뚝’...서울 낮 기온 14도</t>
+          <t>[기상청 전국날씨] 강원영서와 충북북부, 경상권동해안, 경북권내륙 밤까지 비</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>https://www.bntnews.co.kr/article/view/bnt202211130034</t>
+          <t>http://www.pinpointnews.co.kr/news/articleView.html?idxno=154680</t>
         </is>
       </c>
     </row>
@@ -2817,17 +2817,17 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>머니투데이</t>
+          <t>포인트데일리</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>[내일 날씨]비 그치고 찬 바람에 기온 '뚝'…아침 최저 3도</t>
+          <t>[오늘(13일) 날씨] 전국 흐리고 비...오후부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>http://news.mt.co.kr/mtview.php?no=2022111316421114615</t>
+          <t>http://www.thekpm.com/news/articleView.html?idxno=138461</t>
         </is>
       </c>
     </row>
@@ -2839,17 +2839,17 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>시사뉴스</t>
+          <t>톱스타뉴스</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>[내일 날씨] 찬 바람에 아침 쌀쌀...구름 많고 짙은 안개</t>
+          <t>[오늘 전국 날씨] 곳곳 오전까지 비 소식…오후부터 기온 '뚝'</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>https://www.sisa-news.com/news/article.html?no=220272</t>
+          <t>http://www.topstarnews.net/news/articleView.html?idxno=14778243</t>
         </is>
       </c>
     </row>
@@ -2861,17 +2861,17 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>이코노뉴스</t>
+          <t>SR타임스</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>[내일 날씨] 월요일 아침 북서쪽에서 찬 공기 유입 '쌀쌀'…구름 많고 안개</t>
+          <t>[오늘 날씨 및 내일 날씨] 가을비 그친 뒤 기온 뚝↓...서울 최저기온 9도...종일 찬바람</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>http://www.econonews.co.kr/news/articleView.html?idxno=266302</t>
+          <t>http://www.srtimes.kr/news/articleView.html?idxno=123576</t>
         </is>
       </c>
     </row>
@@ -2883,17 +2883,17 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>뉴스웍스</t>
+          <t>뉴시스</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>[내일 날씨] 전국 구름 많고 추워…아침 최저 3도</t>
+          <t>찬공기 유입에 내일 아침 쌀쌀…구름 많고 안개</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>http://www.newsworks.co.kr/news/articleView.html?idxno=614961</t>
+          <t>http://www.newsis.com/view/?id=NISX20221113_0002084142&amp;cID=10201&amp;pID=10200</t>
         </is>
       </c>
     </row>
@@ -2905,17 +2905,17 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>열린뉴스통신</t>
+          <t>세계일보</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>[내일날씨] 찬 공기 남하하며 아침 기온 '뚝'…강풍에 체감 온도↓</t>
+          <t>[내일날씨] 전국 구름 많은 가운데 13일보다 5∼10도 더 떨어져</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>https://www.onews.tv/news/articleView.html?idxno=144131</t>
+          <t>http://www.segye.com/content/html/2022/11/13/20221113508264.html?OutUrl=naver</t>
         </is>
       </c>
     </row>
@@ -2927,17 +2927,17 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>한스경제</t>
+          <t>머니S</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>[내일날씨] 출근길 짙은 안개... 찬 공기에 건강 주의</t>
+          <t>[내일 날씨] 전국 구름 많고 기온 '뚝'… 서울 최고기온 14도</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>http://www.sporbiz.co.kr/news/articleView.html?idxno=637619</t>
+          <t>http://moneys.mt.co.kr/news/mwView.php?no=2022111315372838730</t>
         </is>
       </c>
     </row>
@@ -2949,17 +2949,325 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
+          <t>bnt뉴스</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>내일날씨, 찬 바람 기온 ‘뚝’...서울 낮 기온 14도</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>https://www.bntnews.co.kr/article/view/bnt202211130034</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>머니투데이</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>[내일 날씨]비 그치고 찬 바람에 기온 '뚝'…아침 최저 3도</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>http://news.mt.co.kr/mtview.php?no=2022111316421114615</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>시사뉴스</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>[내일 날씨] 찬 바람에 아침 쌀쌀...구름 많고 짙은 안개</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>https://www.sisa-news.com/news/article.html?no=220272</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>이코노뉴스</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>[내일 날씨] 월요일 아침 북서쪽에서 찬 공기 유입 '쌀쌀'…구름 많고 안개</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>http://www.econonews.co.kr/news/articleView.html?idxno=266302</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>뉴스웍스</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>[내일 날씨] 전국 구름 많고 추워…아침 최저 3도</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>http://www.newsworks.co.kr/news/articleView.html?idxno=614961</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>열린뉴스통신</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>[내일날씨] 찬 공기 남하하며 아침 기온 '뚝'…강풍에 체감 온도↓</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>https://www.onews.tv/news/articleView.html?idxno=144131</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>한스경제</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>[내일날씨] 출근길 짙은 안개... 찬 공기에 건강 주의</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>http://www.sporbiz.co.kr/news/articleView.html?idxno=637619</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
           <t>톱스타뉴스</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr">
+      <c r="C122" t="inlineStr">
         <is>
           <t>[내일 전국 날씨] 찬공기 유입에 내일 아침 쌀쌀…구름 많고 안개</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr">
+      <c r="D122" t="inlineStr">
         <is>
           <t>http://www.topstarnews.net/news/articleView.html?idxno=14778464</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>뉴시스</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>추수 끝나면 버려지는 농촌 폐비닐…"한달간 집중수거"</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>http://www.newsis.com/view/?id=NISX20221112_0002083603&amp;cID=10201&amp;pID=10200</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>뉴스1</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>환경부, 내달 중순까지 폐비닐·폐농약용기 등 영농폐기물 집중 수거</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>https://www.news1.kr/articles/4862310</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>헤럴드경제</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>민관 합동으로 영농폐기물 집중 수거한다</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>http://news.heraldcorp.com/view.php?ud=20221113000040</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>이데일리</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>영농폐기물 집중수거기간 한달간 운영…우수 지자체 포상</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>http://www.edaily.co.kr/news/newspath.asp?newsid=01436646632525392</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>이투데이</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>영농 폐비닐 수거보상금 지원단가 kg당 10→20원으로 인상</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>https://www.etoday.co.kr/news/view/2191814</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>전자신문</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>민관, 영농폐기물 집중 수거…“보상금 확대, 재활용시설 확충”</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>https://www.etnews.com/20221113000027</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2022.11.13</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>데일리안</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>환경부, 내달 16일까지 방치된 폐비닐·폐농약용기 집중 수거</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>https://www.dailian.co.kr/news/view/1172571/?sc=Naver</t>
         </is>
       </c>
     </row>

</xml_diff>